<commit_message>
2.0.4: Enable new targetStyle option and lineSeparator option.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoConstantsConstants.xlsx
+++ b/meta/program/BlancoConstantsConstants.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoConstants/meta/program/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75DE123-6D53-7844-B4C3-48045E08B616}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15450" windowHeight="8190" tabRatio="640"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="18520" windowHeight="14740" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -30,12 +36,22 @@
     <definedName name="項目型">#REF!</definedName>
     <definedName name="必須">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
   <si>
     <t>パッケージ</t>
   </si>
@@ -239,13 +255,77 @@
   <si>
     <t>"2.0.1"</t>
     <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>TARGET_STYLE_BLANCO</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>java.lang.String</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>"blanco"</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>targetdirに設定される文字列</t>
+    <rPh sb="10" eb="12">
+      <t xml:space="preserve">セッテイ </t>
+    </rPh>
+    <rPh sb="15" eb="18">
+      <t xml:space="preserve">モジレツ </t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>TARGET_STYLE_MAVEN</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>"maven"</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>TARGET_STYLE_FREE</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>"free"</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>TARGET_DIR_SUFFIX_BLANCO</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>"main"</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>生成したソースコードを保管するディレクトリのsuffix</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">セイセイ </t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t xml:space="preserve">ホカンスル </t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>TARGET_DIR_SUFFIX_MAVEN</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>"main/java"</t>
+    <phoneticPr fontId="6"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -274,6 +354,18 @@
       <sz val="6"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="ＭＳ ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
       <charset val="128"/>
     </font>
   </fonts>
@@ -625,7 +717,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -735,17 +827,31 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="valueObject"/>
@@ -817,7 +923,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -849,9 +955,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -883,6 +1007,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1058,29 +1200,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.75" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="32" style="1" customWidth="1"/>
-    <col min="7" max="7" width="33.375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="33.33203125" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75">
+    <row r="1" spans="1:6" ht="19">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -1277,6 +1419,7 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="41">
+        <f>A20+1</f>
         <v>2</v>
       </c>
       <c r="B21" s="30" t="s">
@@ -1297,6 +1440,7 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="41">
+        <f t="shared" ref="A22:A28" si="0">A21+1</f>
         <v>3</v>
       </c>
       <c r="B22" s="30" t="s">
@@ -1317,6 +1461,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="41">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B23" s="30" t="s">
@@ -1336,51 +1481,106 @@
       <c r="H23"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="41"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
+      <c r="A24" s="41">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B24" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="48" t="s">
+        <v>44</v>
+      </c>
       <c r="F24" s="35"/>
       <c r="G24"/>
       <c r="H24"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="41"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
+      <c r="A25" s="41">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B25" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="48" t="s">
+        <v>44</v>
+      </c>
       <c r="F25" s="35"/>
       <c r="G25"/>
       <c r="H25"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="41"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
+      <c r="A26" s="41">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B26" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="48" t="s">
+        <v>44</v>
+      </c>
       <c r="F26" s="35"/>
       <c r="G26"/>
       <c r="H26"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="41"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
+      <c r="A27" s="41">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B27" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="48" t="s">
+        <v>51</v>
+      </c>
       <c r="F27" s="35"/>
       <c r="G27"/>
       <c r="H27"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="42"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
+      <c r="A28" s="41">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B28" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="48" t="s">
+        <v>51</v>
+      </c>
       <c r="F28" s="37"/>
       <c r="G28"/>
       <c r="H28"/>
@@ -1433,17 +1633,17 @@
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D47">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D47" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>adjustConstValue</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>isAbstract</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>accessScope</formula1>
     </dataValidation>
   </dataValidations>
@@ -1456,20 +1656,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="2" max="2" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75">
+    <row r="1" spans="1:10" ht="19">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>

</xml_diff>